<commit_message>
added cases to booking.com
</commit_message>
<xml_diff>
--- a/com.booking/src/test/resources/test_data.xlsx
+++ b/com.booking/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.booking\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1524062D-1DE0-4AA6-9E9E-7C96C49A92BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3EC89B-E5B6-452F-AD48-009BB11BEE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="2680" yWindow="0" windowWidth="17140" windowHeight="14320" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Assertions</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>New York State</t>
+  </si>
+  <si>
+    <t>Greater London</t>
+  </si>
+  <si>
+    <t>Ile de France</t>
+  </si>
+  <si>
+    <t>Community of Madrid</t>
+  </si>
+  <si>
+    <t>Ohio</t>
   </si>
 </sst>
 </file>
@@ -403,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,6 +441,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added test cases to booking.com
</commit_message>
<xml_diff>
--- a/com.booking/src/test/resources/test_data.xlsx
+++ b/com.booking/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.booking\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3EC89B-E5B6-452F-AD48-009BB11BEE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A3D4E5-0AD3-4437-A22D-C4D1FE37D16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="0" windowWidth="17140" windowHeight="14320" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
@@ -35,27 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Assertions</t>
   </si>
   <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>New York State</t>
-  </si>
-  <si>
-    <t>Greater London</t>
-  </si>
-  <si>
-    <t>Ile de France</t>
-  </si>
-  <si>
-    <t>Community of Madrid</t>
-  </si>
-  <si>
-    <t>Ohio</t>
+    <t>Stays</t>
   </si>
 </sst>
 </file>
@@ -418,7 +403,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,33 +418,23 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>